<commit_message>
checking in edits to the notebook
</commit_message>
<xml_diff>
--- a/single-well-assay/20180402_kinase_panel_HT_single_well_binding_data/040218_Kinase_dispensing_for_binding_assay.xlsx
+++ b/single-well-assay/20180402_kinase_panel_HT_single_well_binding_data/040218_Kinase_dispensing_for_binding_assay.xlsx
@@ -321,10 +321,10 @@
     <t>Buffer</t>
   </si>
   <si>
-    <t>MK14</t>
-  </si>
-  <si>
     <t>boiled MK14</t>
+  </si>
+  <si>
+    <t>control MK14</t>
   </si>
 </sst>
 </file>
@@ -803,7 +803,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1246,7 +1246,7 @@
         <v>69</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1254,7 +1254,7 @@
         <v>70</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:6">

</xml_diff>